<commit_message>
Đang sửa Excel cho thị trường tất cả
</commit_message>
<xml_diff>
--- a/DongAERP/Content/Report/ReportDetailtgradationByMakets.xlsx
+++ b/DongAERP/Content/Report/ReportDetailtgradationByMakets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\DongAERP\DongAERP\DongAERP\Content\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5680D2-AE9A-49B6-85FA-CEF64710A326}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2222DF38-ECF0-4E7F-87B6-9A4E33275A8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FDADBC8A-6B6C-45FD-98E5-87326587A42E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Từ:</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>Chuyển khoản</t>
-  </si>
-  <si>
-    <t>1. Theo doanh số chi trả theo thị trường - loại hình chi trả</t>
   </si>
 </sst>
 </file>
@@ -166,15 +163,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,13 +489,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C3B6D35-F82E-4989-A479-5B01F28891A5}">
   <dimension ref="A1:W44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
     <col min="3" max="3" width="19.44140625" customWidth="1"/>
     <col min="4" max="4" width="17.77734375" customWidth="1"/>
     <col min="5" max="5" width="17.109375" customWidth="1"/>
@@ -607,12 +604,10 @@
     </row>
     <row r="7" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
-      <c r="B7" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="P7" s="7"/>
@@ -626,461 +621,461 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
       <c r="P8" s="4"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
       <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
       <c r="P10" s="4"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
       <c r="P11" s="4"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
       <c r="P12" s="4"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
       <c r="P13" s="4"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
       <c r="P14" s="4"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
       <c r="P15" s="4"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
       <c r="P16" s="4"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
       <c r="P17" s="4"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
       <c r="P18" s="4"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
       <c r="P19" s="4"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
       <c r="P20" s="4"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
       <c r="P21" s="4"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
       <c r="P22" s="4"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
       <c r="P23" s="4"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
       <c r="P24" s="4"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.3">
       <c r="P25" s="4"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="16"/>
-      <c r="O26" s="16"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="16"/>
-      <c r="O27" s="16"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="16"/>
-      <c r="O28" s="16"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
-      <c r="O29" s="16"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="16"/>
-      <c r="O30" s="16"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
-      <c r="L31" s="16"/>
-      <c r="M31" s="16"/>
-      <c r="N31" s="16"/>
-      <c r="O31" s="16"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="16"/>
-      <c r="L32" s="16"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="16"/>
-      <c r="O32" s="16"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="16"/>
-      <c r="L33" s="16"/>
-      <c r="M33" s="16"/>
-      <c r="N33" s="16"/>
-      <c r="O33" s="16"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="16"/>
-      <c r="N34" s="16"/>
-      <c r="O34" s="16"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="L35" s="16"/>
-      <c r="M35" s="16"/>
-      <c r="N35" s="16"/>
-      <c r="O35" s="16"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="16"/>
-      <c r="L36" s="16"/>
-      <c r="M36" s="16"/>
-      <c r="N36" s="16"/>
-      <c r="O36" s="16"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B37" s="16"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="16"/>
-      <c r="L37" s="16"/>
-      <c r="M37" s="16"/>
-      <c r="N37" s="16"/>
-      <c r="O37" s="16"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="16"/>
-      <c r="L38" s="16"/>
-      <c r="M38" s="16"/>
-      <c r="N38" s="16"/>
-      <c r="O38" s="16"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="16"/>
-      <c r="L39" s="16"/>
-      <c r="M39" s="16"/>
-      <c r="N39" s="16"/>
-      <c r="O39" s="16"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
+      <c r="O39" s="15"/>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
-      <c r="I40" s="16"/>
-      <c r="J40" s="16"/>
-      <c r="L40" s="16"/>
-      <c r="M40" s="16"/>
-      <c r="N40" s="16"/>
-      <c r="O40" s="16"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B43" s="17"/>
-      <c r="C43" s="18" t="s">
+      <c r="B43" s="16"/>
+      <c r="C43" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18" t="s">
+      <c r="D43" s="17"/>
+      <c r="E43" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18" t="s">
+      <c r="F43" s="17"/>
+      <c r="G43" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18" t="s">
+      <c r="H43" s="17"/>
+      <c r="I43" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="J43" s="18"/>
+      <c r="J43" s="17"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B44" s="17"/>
+      <c r="B44" s="16"/>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
@@ -1091,10 +1086,9 @@
       <c r="J44" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B43:B44"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="E43:F43"/>

</xml_diff>

<commit_message>
Đang làm thị trường chi tiết 1 thị trường
</commit_message>
<xml_diff>
--- a/DongAERP/Content/Report/ReportDetailtgradationByMakets.xlsx
+++ b/DongAERP/Content/Report/ReportDetailtgradationByMakets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DongAERP\DongAERP\Content\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC7F502-203D-4146-BCBE-8A5FDD2CF319}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226AF98E-A68C-4497-8B79-2E7F669E3F64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FDADBC8A-6B6C-45FD-98E5-87326587A42E}"/>
   </bookViews>
@@ -41,12 +41,6 @@
     <t>BÁO CÁO TỔNG HỢP - THEO TỪNG THỊ TRƯỜNG</t>
   </si>
   <si>
-    <t>Chi nhà</t>
-  </si>
-  <si>
-    <t>Chi quầy</t>
-  </si>
-  <si>
     <t>Chuyển khoản</t>
   </si>
   <si>
@@ -54,6 +48,12 @@
   </si>
   <si>
     <t>USD</t>
+  </si>
+  <si>
+    <t>Chi Nhà</t>
+  </si>
+  <si>
+    <t>Chi Quầy</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
   <dimension ref="A1:W62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66"/>
+      <selection activeCell="C61" sqref="C61:D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1114,24 +1114,24 @@
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I60" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J60" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B61" s="16"/>
       <c r="C61" s="17" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D61" s="17"/>
       <c r="E61" s="17" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F61" s="17"/>
       <c r="G61" s="17" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H61" s="17"/>
       <c r="I61" s="17" t="s">

</xml_diff>